<commit_message>
add files in lenga-patagonia
</commit_message>
<xml_diff>
--- a/web-lenga/reporte_resumen_trimestral.xlsx
+++ b/web-lenga/reporte_resumen_trimestral.xlsx
@@ -471,16 +471,16 @@
         <v>43831</v>
       </c>
       <c r="B2" t="n">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C2" t="n">
-        <v>134</v>
+        <v>103</v>
       </c>
       <c r="D2" t="n">
-        <v>94</v>
+        <v>71</v>
       </c>
       <c r="E2" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -505,16 +505,16 @@
         <v>44197</v>
       </c>
       <c r="B4" t="n">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>298</v>
+        <v>20</v>
       </c>
       <c r="D4" t="n">
-        <v>179</v>
+        <v>9</v>
       </c>
       <c r="E4" t="n">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -522,16 +522,16 @@
         <v>44287</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="D5" t="n">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="E5" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6">
@@ -556,16 +556,16 @@
         <v>44470</v>
       </c>
       <c r="B7" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D7" t="n">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="E7" t="n">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
@@ -576,7 +576,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="n">
         <v>59</v>
@@ -593,10 +593,10 @@
         <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -613,10 +613,10 @@
         <v>113</v>
       </c>
       <c r="D10" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E10" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11">
@@ -624,16 +624,16 @@
         <v>44835</v>
       </c>
       <c r="B11" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" t="n">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="D11" t="n">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="E11" t="n">
-        <v>50</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12">
@@ -647,10 +647,10 @@
         <v>127</v>
       </c>
       <c r="D12" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -661,13 +661,13 @@
         <v>15</v>
       </c>
       <c r="C13" t="n">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D13" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -698,7 +698,7 @@
         <v>59</v>
       </c>
       <c r="D15" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" t="n">
         <v>7</v>
@@ -729,7 +729,7 @@
         <v>25</v>
       </c>
       <c r="C17" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D17" t="n">
         <v>48</v>

</xml_diff>